<commit_message>
started combining model + visual
</commit_message>
<xml_diff>
--- a/data/case6ww.xlsx
+++ b/data/case6ww.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99A4DA37-2C99-43DF-9D9E-C00407EEC428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bus" sheetId="1" r:id="rId1"/>
@@ -19,12 +25,12 @@
     <sheet name="timeseries" sheetId="10" r:id="rId10"/>
     <sheet name="baseMVA" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="126">
   <si>
     <t>name</t>
   </si>
@@ -393,13 +399,22 @@
   </si>
   <si>
     <t>baseMVA</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>storage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,7 +439,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -447,13 +462,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -462,13 +494,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -506,7 +546,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -540,6 +580,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -574,9 +615,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -749,14 +791,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -787,8 +831,17 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -819,8 +872,17 @@
       <c r="J2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -851,8 +913,17 @@
       <c r="J3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>7</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -883,8 +954,17 @@
       <c r="J4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -915,8 +995,17 @@
       <c r="J5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -947,8 +1036,17 @@
       <c r="J6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="K6">
+        <v>5</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -978,6 +1076,15 @@
       </c>
       <c r="J7" t="s">
         <v>17</v>
+      </c>
+      <c r="K7">
+        <v>6</v>
+      </c>
+      <c r="L7">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -986,31 +1093,31 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>100</v>
       </c>
@@ -1021,14 +1128,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1068,7 +1175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1088,7 +1195,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1108,7 +1215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1128,7 +1235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1148,7 +1255,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1174,14 +1281,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1329,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>45</v>
       </c>
@@ -1263,7 +1370,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>46</v>
       </c>
@@ -1304,7 +1411,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>47</v>
       </c>
@@ -1345,7 +1452,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1386,7 +1493,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1427,7 +1534,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>50</v>
       </c>
@@ -1468,7 +1575,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>51</v>
       </c>
@@ -1509,7 +1616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>52</v>
       </c>
@@ -1550,7 +1657,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>53</v>
       </c>
@@ -1591,7 +1698,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1632,7 +1739,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>55</v>
       </c>
@@ -1679,14 +1786,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1745,14 +1852,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1796,14 +1903,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1826,14 +1933,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1847,14 +1954,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1868,14 +1975,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>21</v>
       </c>
@@ -1946,7 +2053,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2017,7 +2124,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2088,7 +2195,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>12</v>
       </c>

</xml_diff>